<commit_message>
cable loader update + update data generic
</commit_message>
<xml_diff>
--- a/data_ProjectTemplate/Cables_ProjectTemplate.xlsx
+++ b/data_ProjectTemplate/Cables_ProjectTemplate.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Zero_ProjectTemplate\data_ProjectTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\LUX_ProjectTemplate\data_ProjectTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313B05A4-0482-4976-A119-F796113D33C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD253835-F96B-45A3-863D-67670E520A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{F539EAA3-F419-42E2-843D-ACE76198D8F4}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F539EAA3-F419-42E2-843D-ACE76198D8F4}"/>
   </bookViews>
   <sheets>
-    <sheet name="lv_cables" sheetId="5" r:id="rId1"/>
-    <sheet name="mv_cables" sheetId="2" r:id="rId2"/>
+    <sheet name="cables" sheetId="5" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">mv_cables!$A$1:$H$1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -71,7 +67,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{13D5B54F-C6B7-402A-B19E-F8D8F9204816}">
+    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{93E2F9B2-65A4-44F0-A5F4-0CA8281182EF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ate Hempenius:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+(Mandatory) OL_GISObjectType: LV_CABLE, MV_CABLE, etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{13D5B54F-C6B7-402A-B19E-F8D8F9204816}">
       <text>
         <r>
           <rPr>
@@ -97,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{EC85960B-E03A-4685-B845-DA07639BEA50}">
+    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{EC85960B-E03A-4685-B845-DA07639BEA50}">
       <text>
         <r>
           <rPr>
@@ -122,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{F2F1AA96-1129-4DF1-B3B2-523D8402B6DE}">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{F2F1AA96-1129-4DF1-B3B2-523D8402B6DE}">
       <text>
         <r>
           <rPr>
@@ -147,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{BB0BF842-CEF4-4C26-90CD-B766A3AD3519}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{BB0BF842-CEF4-4C26-90CD-B766A3AD3519}">
       <text>
         <r>
           <rPr>
@@ -172,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E9B5C156-B0FA-42E8-826C-1216D442E8E9}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{E9B5C156-B0FA-42E8-826C-1216D442E8E9}">
       <text>
         <r>
           <rPr>
@@ -196,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{E8BD55DF-BD1B-4361-A7AB-4C69AF2D52B6}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{E8BD55DF-BD1B-4361-A7AB-4C69AF2D52B6}">
       <text>
         <r>
           <rPr>
@@ -220,218 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{74EE1F63-13A1-4325-B8E5-506BBAE22FED}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Luc Sol:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-String (mandatory)
-Line coordinates from qgis
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Luc Sol</author>
-    <author>Ate Hempenius</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CB8C1CC1-A71D-416D-9F95-1F33E06F1407}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Luc Sol:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-String (optional)
-id from QGIS</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{4EF939E2-3185-496E-AD0E-CE714B9C152D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Luc Sol:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Boolean (mandatory)
-TRUE if the cable is part of the model. FALSE otherwise
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{A4292159-885E-421F-9824-5B0A6AE2B8FD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ate Hempenius:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-double (optional for now)
-nominal voltage of the cable [V]</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{E295CD28-EA76-44D3-A01D-046FDDB7D5B9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ate Hempenius:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-string (optional)
-cable group of the gridoperator (identifier could be usefull)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{7526DE32-75D7-4A1D-BFE2-61DD9CD70254}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Luc Sol:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-String (optional)
-Information about the type of cable (goal)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{8D642436-AE55-4E9A-B4C4-257A05FA024F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Luc Sol:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-double (mandatory)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{111595BC-A3E5-457A-B018-2F84EE120EF6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Luc Sol:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-double (mandatory)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{BE32E3F2-17EC-443A-AD2A-79E23CB09F67}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{74EE1F63-13A1-4325-B8E5-506BBAE22FED}">
       <text>
         <r>
           <rPr>
@@ -462,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>fid</t>
   </si>
@@ -486,6 +295,9 @@
   </si>
   <si>
     <t>nominal_voltage_v</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -556,27 +368,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -927,103 +719,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA96489D-AFDF-4D44-8F24-6A3D55626B5B}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B02188-73B1-498C-8C13-7E9E7FF97634}">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A1:B1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1">
+  <conditionalFormatting sqref="C1">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>